<commit_message>
Updates on cost assumption
</commit_message>
<xml_diff>
--- a/Model and input data/Input_Data/Cost_assumptions/MASTER_PGP_system_costs_08July2021.xlsx
+++ b/Model and input data/Input_Data/Cost_assumptions/MASTER_PGP_system_costs_08July2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacquelinedowling/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leiduan/Desktop/File/Research/GitKraken_Repository/Advanced_nuclear_2021/Model and input data/Input_Data/Cost_assumptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3C5AD7-EFDA-0240-BD0A-2FD7F2BB3F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39466464-4D57-EF43-9437-1F8B3B03200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="1260" windowWidth="20460" windowHeight="16000" xr2:uid="{9402D557-0539-F249-9981-FEF30EBBF85E}"/>
+    <workbookView xWindow="31040" yWindow="-3480" windowWidth="27280" windowHeight="24800" xr2:uid="{9402D557-0539-F249-9981-FEF30EBBF85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D89738-6C80-4948-ACFD-8AF97CD34964}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1278,7 +1278,7 @@
         <v>6.8590905054270843</v>
       </c>
       <c r="G24" s="8" t="e">
-        <f t="shared" ref="G24:I24" si="1">G23/G20</f>
+        <f t="shared" ref="G24:H24" si="1">G23/G20</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H24" s="8" t="e">
@@ -1413,7 +1413,7 @@
         <v>623067.42000000004</v>
       </c>
       <c r="G29" s="14">
-        <f t="shared" ref="G29:J29" si="5">G27*D14</f>
+        <f t="shared" ref="G29:H29" si="5">G27*D14</f>
         <v>0</v>
       </c>
       <c r="H29" s="14">
@@ -1492,27 +1492,27 @@
         <v>1.1212276062325208</v>
       </c>
       <c r="E32" s="22">
-        <f>E31/HOURS_PER_YEAR</f>
+        <f t="shared" ref="E32:J32" si="7">E31/HOURS_PER_YEAR</f>
         <v>3.2302820402436073E-2</v>
       </c>
       <c r="F32" s="23">
-        <f>F31/HOURS_PER_YEAR</f>
+        <f t="shared" si="7"/>
         <v>1.2442406240398258E-4</v>
       </c>
       <c r="G32" s="15">
-        <f>G31/HOURS_PER_YEAR</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H32" s="15">
-        <f>H31/HOURS_PER_YEAR</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I32" s="23">
-        <f>I31/HOURS_PER_YEAR</f>
+        <f t="shared" si="7"/>
         <v>0.21592975742129025</v>
       </c>
       <c r="J32" s="23">
-        <f>J31/HOURS_PER_YEAR</f>
+        <f t="shared" si="7"/>
         <v>5.8463933229736795E-2</v>
       </c>
     </row>

</xml_diff>